<commit_message>
remove negative cross sections
</commit_message>
<xml_diff>
--- a/proton_qT/expdata/12881.xlsx
+++ b/proton_qT/expdata/12881.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/proton_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA915AF2-753A-9C4E-A73E-15A86600FD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756827FD-7F04-0446-BC76-FBCBE7348ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="8620" windowWidth="27240" windowHeight="11100" xr2:uid="{36F8C7AD-8A08-4C4F-859F-62114E017E0C}"/>
+    <workbookView xWindow="2080" yWindow="2600" windowWidth="28680" windowHeight="18560" xr2:uid="{36F8C7AD-8A08-4C4F-859F-62114E017E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="19">
   <si>
     <t>value</t>
   </si>
@@ -466,11 +466,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901D04B3-5AA6-704E-B05A-2C52B3F08299}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -607,7 +605,7 @@
         <v>0.24</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K66" si="0">0.25*I3</f>
+        <f t="shared" ref="K3:K63" si="0">0.25*I3</f>
         <v>1.47</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1036,10 +1034,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="E13" s="2">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>5</v>
@@ -1051,14 +1049,14 @@
         <v>11</v>
       </c>
       <c r="I13" s="3">
-        <v>-3.3000000000000002E-2</v>
+        <v>0.10500000000000001</v>
       </c>
       <c r="J13" s="3">
-        <v>5.5E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
-        <v>-8.2500000000000004E-3</v>
+        <v>2.6250000000000002E-2</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>10</v>
@@ -1075,16 +1073,16 @@
         <v>200</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>2.6</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>5</v>
@@ -1096,14 +1094,14 @@
         <v>11</v>
       </c>
       <c r="I14" s="3">
-        <v>0.10500000000000001</v>
+        <v>1.63</v>
       </c>
       <c r="J14" s="3">
-        <v>5.6000000000000001E-2</v>
+        <v>0.11</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="0"/>
-        <v>2.6250000000000002E-2</v>
+        <v>0.40749999999999997</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>10</v>
@@ -1120,16 +1118,16 @@
         <v>200</v>
       </c>
       <c r="B15" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>2.6</v>
+        <v>0.2</v>
       </c>
       <c r="E15" s="2">
-        <v>2.8</v>
+        <v>0.4</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>5</v>
@@ -1141,14 +1139,14 @@
         <v>11</v>
       </c>
       <c r="I15" s="3">
-        <v>-7.3000000000000009E-2</v>
+        <v>1.4400000000000002</v>
       </c>
       <c r="J15" s="3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.08</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>-1.8250000000000002E-2</v>
+        <v>0.36000000000000004</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>10</v>
@@ -1171,10 +1169,10 @@
         <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E16" s="2">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>5</v>
@@ -1186,14 +1184,14 @@
         <v>11</v>
       </c>
       <c r="I16" s="3">
-        <v>1.63</v>
+        <v>1.19</v>
       </c>
       <c r="J16" s="3">
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="3">
         <f t="shared" si="0"/>
-        <v>0.40749999999999997</v>
+        <v>0.29749999999999999</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>10</v>
@@ -1216,10 +1214,10 @@
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E17" s="2">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>5</v>
@@ -1231,14 +1229,14 @@
         <v>11</v>
       </c>
       <c r="I17" s="3">
-        <v>1.4400000000000002</v>
+        <v>1.04</v>
       </c>
       <c r="J17" s="3">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>0.36000000000000004</v>
+        <v>0.26</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>10</v>
@@ -1261,10 +1259,10 @@
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E18" s="2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>5</v>
@@ -1276,14 +1274,14 @@
         <v>11</v>
       </c>
       <c r="I18" s="3">
-        <v>1.19</v>
+        <v>0.60100000000000009</v>
       </c>
       <c r="J18" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="K18" s="3">
         <f t="shared" si="0"/>
-        <v>0.29749999999999999</v>
+        <v>0.15025000000000002</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>10</v>
@@ -1306,10 +1304,10 @@
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>5</v>
@@ -1321,14 +1319,14 @@
         <v>11</v>
       </c>
       <c r="I19" s="3">
-        <v>1.04</v>
+        <v>0.44100000000000006</v>
       </c>
       <c r="J19" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>4.3000000000000003E-2</v>
       </c>
       <c r="K19" s="3">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.11025000000000001</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>10</v>
@@ -1351,10 +1349,10 @@
         <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
@@ -1366,14 +1364,14 @@
         <v>11</v>
       </c>
       <c r="I20" s="3">
-        <v>0.60100000000000009</v>
+        <v>0.248</v>
       </c>
       <c r="J20" s="3">
-        <v>5.1000000000000004E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="0"/>
-        <v>0.15025000000000002</v>
+        <v>6.2E-2</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>10</v>
@@ -1396,10 +1394,10 @@
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="E21" s="2">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
@@ -1411,14 +1409,14 @@
         <v>11</v>
       </c>
       <c r="I21" s="3">
-        <v>0.44100000000000006</v>
+        <v>0.255</v>
       </c>
       <c r="J21" s="3">
-        <v>4.3000000000000003E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="0"/>
-        <v>0.11025000000000001</v>
+        <v>6.3750000000000001E-2</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>10</v>
@@ -1441,10 +1439,10 @@
         <v>6</v>
       </c>
       <c r="D22" s="2">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="E22" s="2">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
@@ -1456,14 +1454,14 @@
         <v>11</v>
       </c>
       <c r="I22" s="3">
-        <v>0.248</v>
+        <v>0.159</v>
       </c>
       <c r="J22" s="3">
-        <v>0.03</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" si="0"/>
-        <v>6.2E-2</v>
+        <v>3.9750000000000001E-2</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>10</v>
@@ -1486,10 +1484,10 @@
         <v>6</v>
       </c>
       <c r="D23" s="2">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="E23" s="2">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -1501,14 +1499,14 @@
         <v>11</v>
       </c>
       <c r="I23" s="3">
-        <v>0.255</v>
+        <v>6.3E-2</v>
       </c>
       <c r="J23" s="3">
-        <v>3.6000000000000004E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="0"/>
-        <v>6.3750000000000001E-2</v>
+        <v>1.575E-2</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>10</v>
@@ -1531,10 +1529,10 @@
         <v>6</v>
       </c>
       <c r="D24" s="2">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2">
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -1546,14 +1544,14 @@
         <v>11</v>
       </c>
       <c r="I24" s="3">
-        <v>0.159</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="J24" s="3">
-        <v>2.8000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="0"/>
-        <v>3.9750000000000001E-2</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>10</v>
@@ -1576,10 +1574,10 @@
         <v>6</v>
       </c>
       <c r="D25" s="2">
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E25" s="2">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>5</v>
@@ -1591,14 +1589,14 @@
         <v>11</v>
       </c>
       <c r="I25" s="3">
-        <v>6.3E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J25" s="3">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="0"/>
-        <v>1.575E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>10</v>
@@ -1621,10 +1619,10 @@
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="E26" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>5</v>
@@ -1636,14 +1634,14 @@
         <v>11</v>
       </c>
       <c r="I26" s="3">
-        <v>4.4000000000000004E-2</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="J26" s="3">
-        <v>1.6E-2</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="K26" s="3">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-2</v>
+        <v>2.0250000000000003E-3</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>10</v>
@@ -1666,10 +1664,10 @@
         <v>6</v>
       </c>
       <c r="D27" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="E27" s="2">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>5</v>
@@ -1681,14 +1679,14 @@
         <v>11</v>
       </c>
       <c r="I27" s="3">
-        <v>0.05</v>
+        <v>1.18E-2</v>
       </c>
       <c r="J27" s="3">
-        <v>1.6E-2</v>
+        <v>8.7000000000000011E-3</v>
       </c>
       <c r="K27" s="3">
         <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <v>2.9499999999999999E-3</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>10</v>
@@ -1711,10 +1709,10 @@
         <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="E28" s="2">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>5</v>
@@ -1726,14 +1724,14 @@
         <v>11</v>
       </c>
       <c r="I28" s="3">
-        <v>8.1000000000000013E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="J28" s="3">
-        <v>8.3000000000000001E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="0"/>
-        <v>2.0250000000000003E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>10</v>
@@ -1750,16 +1748,16 @@
         <v>200</v>
       </c>
       <c r="B29" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2">
-        <v>2.8</v>
+        <v>0.2</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>5</v>
@@ -1771,14 +1769,14 @@
         <v>11</v>
       </c>
       <c r="I29" s="3">
-        <v>1.18E-2</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="J29" s="3">
-        <v>8.7000000000000011E-3</v>
+        <v>4.3000000000000003E-2</v>
       </c>
       <c r="K29" s="3">
         <f t="shared" si="0"/>
-        <v>2.9499999999999999E-3</v>
+        <v>9.9750000000000005E-2</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>10</v>
@@ -1795,16 +1793,16 @@
         <v>200</v>
       </c>
       <c r="B30" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2">
-        <v>2.8</v>
+        <v>0.2</v>
       </c>
       <c r="E30" s="2">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>5</v>
@@ -1816,14 +1814,14 @@
         <v>11</v>
       </c>
       <c r="I30" s="3">
-        <v>4.1999999999999997E-3</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="J30" s="3">
-        <v>4.1999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K30" s="3">
         <f t="shared" si="0"/>
-        <v>1.0499999999999999E-3</v>
+        <v>8.5500000000000007E-2</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>10</v>
@@ -1840,16 +1838,16 @@
         <v>200</v>
       </c>
       <c r="B31" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2">
-        <v>3.2</v>
+        <v>0.4</v>
       </c>
       <c r="E31" s="2">
-        <v>3.4</v>
+        <v>0.6</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>5</v>
@@ -1861,14 +1859,14 @@
         <v>11</v>
       </c>
       <c r="I31" s="3">
-        <v>-5.0000000000000001E-3</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="J31" s="3">
-        <v>5.1000000000000004E-3</v>
+        <v>2.2000000000000002E-2</v>
       </c>
       <c r="K31" s="3">
         <f t="shared" si="0"/>
-        <v>-1.25E-3</v>
+        <v>8.3250000000000005E-2</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>10</v>
@@ -1891,10 +1889,10 @@
         <v>7</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E32" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>5</v>
@@ -1906,14 +1904,14 @@
         <v>11</v>
       </c>
       <c r="I32" s="3">
-        <v>0.39900000000000002</v>
+        <v>0.255</v>
       </c>
       <c r="J32" s="3">
-        <v>4.3000000000000003E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K32" s="3">
         <f t="shared" si="0"/>
-        <v>9.9750000000000005E-2</v>
+        <v>6.3750000000000001E-2</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>10</v>
@@ -1936,10 +1934,10 @@
         <v>7</v>
       </c>
       <c r="D33" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E33" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>5</v>
@@ -1951,14 +1949,14 @@
         <v>11</v>
       </c>
       <c r="I33" s="3">
-        <v>0.34200000000000003</v>
+        <v>0.18100000000000002</v>
       </c>
       <c r="J33" s="3">
-        <v>2.5000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K33" s="3">
         <f t="shared" si="0"/>
-        <v>8.5500000000000007E-2</v>
+        <v>4.5250000000000005E-2</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>10</v>
@@ -1981,10 +1979,10 @@
         <v>7</v>
       </c>
       <c r="D34" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E34" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>5</v>
@@ -1996,14 +1994,14 @@
         <v>11</v>
       </c>
       <c r="I34" s="3">
-        <v>0.33300000000000002</v>
+        <v>0.13</v>
       </c>
       <c r="J34" s="3">
-        <v>2.2000000000000002E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K34" s="3">
         <f t="shared" si="0"/>
-        <v>8.3250000000000005E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>10</v>
@@ -2026,10 +2024,10 @@
         <v>7</v>
       </c>
       <c r="D35" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="E35" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>5</v>
@@ -2041,14 +2039,14 @@
         <v>11</v>
       </c>
       <c r="I35" s="3">
-        <v>0.255</v>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="J35" s="3">
-        <v>0.02</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="K35" s="3">
         <f t="shared" si="0"/>
-        <v>6.3750000000000001E-2</v>
+        <v>1.8250000000000002E-2</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>10</v>
@@ -2071,10 +2069,10 @@
         <v>7</v>
       </c>
       <c r="D36" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="E36" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>5</v>
@@ -2086,14 +2084,14 @@
         <v>11</v>
       </c>
       <c r="I36" s="3">
-        <v>0.18100000000000002</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="J36" s="3">
-        <v>1.7000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K36" s="3">
         <f t="shared" si="0"/>
-        <v>4.5250000000000005E-2</v>
+        <v>1.1250000000000001E-2</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>10</v>
@@ -2116,10 +2114,10 @@
         <v>7</v>
       </c>
       <c r="D37" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E37" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>5</v>
@@ -2131,14 +2129,14 @@
         <v>11</v>
       </c>
       <c r="I37" s="3">
-        <v>0.13</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J37" s="3">
-        <v>1.4E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" si="0"/>
-        <v>3.2500000000000001E-2</v>
+        <v>8.7500000000000008E-3</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>10</v>
@@ -2161,10 +2159,10 @@
         <v>7</v>
       </c>
       <c r="D38" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="E38" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>5</v>
@@ -2176,14 +2174,14 @@
         <v>11</v>
       </c>
       <c r="I38" s="3">
-        <v>7.3000000000000009E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J38" s="3">
-        <v>1.1000000000000001E-2</v>
+        <v>6.000000000000001E-3</v>
       </c>
       <c r="K38" s="3">
         <f t="shared" si="0"/>
-        <v>1.8250000000000002E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>10</v>
@@ -2206,10 +2204,10 @@
         <v>7</v>
       </c>
       <c r="D39" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="E39" s="2">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>5</v>
@@ -2221,14 +2219,14 @@
         <v>11</v>
       </c>
       <c r="I39" s="3">
-        <v>4.5000000000000005E-2</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="J39" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="K39" s="3">
         <f t="shared" si="0"/>
-        <v>1.1250000000000001E-2</v>
+        <v>2.075E-3</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>10</v>
@@ -2251,10 +2249,10 @@
         <v>7</v>
       </c>
       <c r="D40" s="2">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E40" s="2">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>5</v>
@@ -2266,14 +2264,14 @@
         <v>11</v>
       </c>
       <c r="I40" s="3">
-        <v>3.5000000000000003E-2</v>
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="J40" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" si="0"/>
-        <v>8.7500000000000008E-3</v>
+        <v>2.3500000000000001E-3</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>10</v>
@@ -2296,10 +2294,10 @@
         <v>7</v>
       </c>
       <c r="D41" s="2">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="E41" s="2">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>5</v>
@@ -2311,14 +2309,14 @@
         <v>11</v>
       </c>
       <c r="I41" s="3">
-        <v>0.02</v>
+        <v>5.3E-3</v>
       </c>
       <c r="J41" s="3">
-        <v>6.000000000000001E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="K41" s="3">
         <f t="shared" si="0"/>
-        <v>5.0000000000000001E-3</v>
+        <v>1.325E-3</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>10</v>
@@ -2341,10 +2339,10 @@
         <v>7</v>
       </c>
       <c r="D42" s="2">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="E42" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>5</v>
@@ -2356,14 +2354,14 @@
         <v>11</v>
       </c>
       <c r="I42" s="3">
-        <v>8.3000000000000001E-3</v>
+        <v>1.8000000000000002E-3</v>
       </c>
       <c r="J42" s="3">
-        <v>3.7000000000000002E-3</v>
+        <v>1.8000000000000002E-3</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="0"/>
-        <v>2.075E-3</v>
+        <v>4.5000000000000004E-4</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>10</v>
@@ -2380,16 +2378,16 @@
         <v>200</v>
       </c>
       <c r="B43" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E43" s="2">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>5</v>
@@ -2401,14 +2399,14 @@
         <v>11</v>
       </c>
       <c r="I43" s="3">
-        <v>9.4000000000000004E-3</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="J43" s="3">
-        <v>4.3E-3</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" si="0"/>
-        <v>2.3500000000000001E-3</v>
+        <v>2.3625E-2</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>10</v>
@@ -2425,16 +2423,16 @@
         <v>200</v>
       </c>
       <c r="B44" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C44" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" s="2">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="E44" s="2">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>5</v>
@@ -2446,14 +2444,14 @@
         <v>11</v>
       </c>
       <c r="I44" s="3">
-        <v>5.3E-3</v>
+        <v>9.0100000000000013E-2</v>
       </c>
       <c r="J44" s="3">
-        <v>3.0999999999999999E-3</v>
+        <v>1.11E-2</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" si="0"/>
-        <v>1.325E-3</v>
+        <v>2.2525000000000003E-2</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>10</v>
@@ -2470,16 +2468,16 @@
         <v>200</v>
       </c>
       <c r="B45" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D45" s="2">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
       <c r="E45" s="2">
-        <v>2.8</v>
+        <v>0.6</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>5</v>
@@ -2491,14 +2489,14 @@
         <v>11</v>
       </c>
       <c r="I45" s="3">
-        <v>1.8000000000000002E-3</v>
+        <v>7.0199999999999999E-2</v>
       </c>
       <c r="J45" s="3">
-        <v>1.8000000000000002E-3</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="K45" s="3">
         <f t="shared" si="0"/>
-        <v>4.5000000000000004E-4</v>
+        <v>1.755E-2</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>10</v>
@@ -2521,10 +2519,10 @@
         <v>8</v>
       </c>
       <c r="D46" s="2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E46" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>5</v>
@@ -2536,14 +2534,14 @@
         <v>11</v>
       </c>
       <c r="I46" s="3">
-        <v>9.4500000000000001E-2</v>
+        <v>5.2199999999999996E-2</v>
       </c>
       <c r="J46" s="3">
-        <v>1.8800000000000001E-2</v>
+        <v>6.9000000000000008E-3</v>
       </c>
       <c r="K46" s="3">
         <f t="shared" si="0"/>
-        <v>2.3625E-2</v>
+        <v>1.3049999999999999E-2</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>10</v>
@@ -2566,10 +2564,10 @@
         <v>8</v>
       </c>
       <c r="D47" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E47" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>5</v>
@@ -2581,14 +2579,14 @@
         <v>11</v>
       </c>
       <c r="I47" s="3">
-        <v>9.0100000000000013E-2</v>
+        <v>4.1100000000000005E-2</v>
       </c>
       <c r="J47" s="3">
-        <v>1.11E-2</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="K47" s="3">
         <f t="shared" si="0"/>
-        <v>2.2525000000000003E-2</v>
+        <v>1.0275000000000001E-2</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>10</v>
@@ -2611,10 +2609,10 @@
         <v>8</v>
       </c>
       <c r="D48" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E48" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>5</v>
@@ -2626,14 +2624,14 @@
         <v>11</v>
       </c>
       <c r="I48" s="3">
-        <v>7.0199999999999999E-2</v>
+        <v>2.9700000000000001E-2</v>
       </c>
       <c r="J48" s="3">
-        <v>8.3999999999999995E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="K48" s="3">
         <f t="shared" si="0"/>
-        <v>1.755E-2</v>
+        <v>7.4250000000000002E-3</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>10</v>
@@ -2656,10 +2654,10 @@
         <v>8</v>
       </c>
       <c r="D49" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="E49" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>5</v>
@@ -2671,14 +2669,14 @@
         <v>11</v>
       </c>
       <c r="I49" s="3">
-        <v>5.2199999999999996E-2</v>
+        <v>1.6400000000000001E-2</v>
       </c>
       <c r="J49" s="3">
-        <v>6.9000000000000008E-3</v>
+        <v>3.8000000000000004E-3</v>
       </c>
       <c r="K49" s="3">
         <f t="shared" si="0"/>
-        <v>1.3049999999999999E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>10</v>
@@ -2701,10 +2699,10 @@
         <v>8</v>
       </c>
       <c r="D50" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="E50" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>5</v>
@@ -2716,14 +2714,14 @@
         <v>11</v>
       </c>
       <c r="I50" s="3">
-        <v>4.1100000000000005E-2</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="J50" s="3">
-        <v>6.1000000000000004E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="K50" s="3">
         <f t="shared" si="0"/>
-        <v>1.0275000000000001E-2</v>
+        <v>2.3749999999999999E-3</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>10</v>
@@ -2746,10 +2744,10 @@
         <v>8</v>
       </c>
       <c r="D51" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E51" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>5</v>
@@ -2761,14 +2759,14 @@
         <v>11</v>
       </c>
       <c r="I51" s="3">
-        <v>2.9700000000000001E-2</v>
+        <v>6.9000000000000008E-3</v>
       </c>
       <c r="J51" s="3">
-        <v>5.4000000000000003E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="K51" s="3">
         <f t="shared" si="0"/>
-        <v>7.4250000000000002E-3</v>
+        <v>1.7250000000000002E-3</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>10</v>
@@ -2791,10 +2789,10 @@
         <v>8</v>
       </c>
       <c r="D52" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="E52" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>5</v>
@@ -2806,14 +2804,14 @@
         <v>11</v>
       </c>
       <c r="I52" s="3">
-        <v>1.6400000000000001E-2</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="J52" s="3">
-        <v>3.8000000000000004E-3</v>
+        <v>1.7000000000000001E-3</v>
       </c>
       <c r="K52" s="3">
         <f t="shared" si="0"/>
-        <v>4.1000000000000003E-3</v>
+        <v>9.2500000000000004E-4</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>10</v>
@@ -2836,10 +2834,10 @@
         <v>8</v>
       </c>
       <c r="D53" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="2">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>5</v>
@@ -2851,14 +2849,14 @@
         <v>11</v>
       </c>
       <c r="I53" s="3">
-        <v>9.4999999999999998E-3</v>
+        <v>3.1999999999999997E-3</v>
       </c>
       <c r="J53" s="3">
-        <v>2.8999999999999998E-3</v>
+        <v>1.9000000000000002E-3</v>
       </c>
       <c r="K53" s="3">
         <f t="shared" si="0"/>
-        <v>2.3749999999999999E-3</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>10</v>
@@ -2881,10 +2879,10 @@
         <v>8</v>
       </c>
       <c r="D54" s="2">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E54" s="2">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>5</v>
@@ -2896,14 +2894,14 @@
         <v>11</v>
       </c>
       <c r="I54" s="3">
-        <v>6.9000000000000008E-3</v>
+        <v>1.5999999999999999E-3</v>
       </c>
       <c r="J54" s="3">
-        <v>2.5000000000000001E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="K54" s="3">
         <f t="shared" si="0"/>
-        <v>1.7250000000000002E-3</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>10</v>
@@ -2926,10 +2924,10 @@
         <v>8</v>
       </c>
       <c r="D55" s="2">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="E55" s="2">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>5</v>
@@ -2941,14 +2939,14 @@
         <v>11</v>
       </c>
       <c r="I55" s="3">
-        <v>3.7000000000000002E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="J55" s="3">
-        <v>1.7000000000000001E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="K55" s="3">
         <f t="shared" si="0"/>
-        <v>9.2500000000000004E-4</v>
+        <v>2.7500000000000002E-4</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>10</v>
@@ -2965,16 +2963,16 @@
         <v>200</v>
       </c>
       <c r="B56" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D56" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E56" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>5</v>
@@ -2986,14 +2984,14 @@
         <v>11</v>
       </c>
       <c r="I56" s="3">
-        <v>3.1999999999999997E-3</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="J56" s="3">
-        <v>1.9000000000000002E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="K56" s="3">
         <f t="shared" si="0"/>
-        <v>7.9999999999999993E-4</v>
+        <v>5.5500000000000002E-3</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>10</v>
@@ -3010,16 +3008,16 @@
         <v>200</v>
       </c>
       <c r="B57" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C57" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D57" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="E57" s="2">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>5</v>
@@ -3031,14 +3029,14 @@
         <v>11</v>
       </c>
       <c r="I57" s="3">
-        <v>1.5999999999999999E-3</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="J57" s="3">
-        <v>1.2000000000000001E-3</v>
+        <v>3.8000000000000004E-3</v>
       </c>
       <c r="K57" s="3">
         <f t="shared" si="0"/>
-        <v>3.9999999999999996E-4</v>
+        <v>4.1250000000000002E-3</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>10</v>
@@ -3055,16 +3053,16 @@
         <v>200</v>
       </c>
       <c r="B58" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C58" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" s="2">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="E58" s="2">
-        <v>3.2</v>
+        <v>0.6</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>5</v>
@@ -3076,14 +3074,14 @@
         <v>11</v>
       </c>
       <c r="I58" s="3">
-        <v>1.1000000000000001E-3</v>
+        <v>1.3400000000000002E-2</v>
       </c>
       <c r="J58" s="3">
-        <v>1.2000000000000001E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="K58" s="3">
         <f t="shared" si="0"/>
-        <v>2.7500000000000002E-4</v>
+        <v>3.3500000000000005E-3</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>10</v>
@@ -3106,10 +3104,10 @@
         <v>9</v>
       </c>
       <c r="D59" s="2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E59" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>5</v>
@@ -3121,14 +3119,14 @@
         <v>11</v>
       </c>
       <c r="I59" s="3">
-        <v>2.2200000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="J59" s="3">
-        <v>7.4999999999999997E-3</v>
+        <v>2.3000000000000004E-3</v>
       </c>
       <c r="K59" s="3">
         <f t="shared" si="0"/>
-        <v>5.5500000000000002E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>10</v>
@@ -3151,10 +3149,10 @@
         <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E60" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>5</v>
@@ -3166,14 +3164,14 @@
         <v>11</v>
       </c>
       <c r="I60" s="3">
-        <v>1.6500000000000001E-2</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="J60" s="3">
-        <v>3.8000000000000004E-3</v>
+        <v>1.7000000000000001E-3</v>
       </c>
       <c r="K60" s="3">
         <f t="shared" si="0"/>
-        <v>4.1250000000000002E-3</v>
+        <v>1.5250000000000001E-3</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>10</v>
@@ -3196,10 +3194,10 @@
         <v>9</v>
       </c>
       <c r="D61" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E61" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>5</v>
@@ -3211,14 +3209,14 @@
         <v>11</v>
       </c>
       <c r="I61" s="3">
-        <v>1.3400000000000002E-2</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="J61" s="3">
-        <v>2.8999999999999998E-3</v>
+        <v>1.5999999999999999E-3</v>
       </c>
       <c r="K61" s="3">
         <f t="shared" si="0"/>
-        <v>3.3500000000000005E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>10</v>
@@ -3241,10 +3239,10 @@
         <v>9</v>
       </c>
       <c r="D62" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="E62" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>5</v>
@@ -3256,14 +3254,14 @@
         <v>11</v>
       </c>
       <c r="I62" s="3">
-        <v>0.01</v>
+        <v>6.000000000000001E-3</v>
       </c>
       <c r="J62" s="3">
-        <v>2.3000000000000004E-3</v>
+        <v>1.8000000000000002E-3</v>
       </c>
       <c r="K62" s="3">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-3</v>
+        <v>1.5000000000000002E-3</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>10</v>
@@ -3286,10 +3284,10 @@
         <v>9</v>
       </c>
       <c r="D63" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="E63" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>5</v>
@@ -3301,14 +3299,14 @@
         <v>11</v>
       </c>
       <c r="I63" s="3">
-        <v>6.1000000000000004E-3</v>
+        <v>1.7000000000000001E-3</v>
       </c>
       <c r="J63" s="3">
-        <v>1.7000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="K63" s="3">
         <f t="shared" si="0"/>
-        <v>1.5250000000000001E-3</v>
+        <v>4.2500000000000003E-4</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>10</v>
@@ -3331,10 +3329,10 @@
         <v>9</v>
       </c>
       <c r="D64" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E64" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>5</v>
@@ -3346,14 +3344,14 @@
         <v>11</v>
       </c>
       <c r="I64" s="3">
-        <v>5.1999999999999998E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="J64" s="3">
-        <v>1.5999999999999999E-3</v>
+        <v>7.5000000000000012E-4</v>
       </c>
       <c r="K64" s="3">
-        <f t="shared" si="0"/>
-        <v>1.2999999999999999E-3</v>
+        <f t="shared" ref="K64:K87" si="1">0.25*I64</f>
+        <v>2.6249999999999998E-4</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>10</v>
@@ -3376,10 +3374,10 @@
         <v>9</v>
       </c>
       <c r="D65" s="2">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="E65" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>5</v>
@@ -3391,14 +3389,14 @@
         <v>11</v>
       </c>
       <c r="I65" s="3">
-        <v>6.000000000000001E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="J65" s="3">
-        <v>1.8000000000000002E-3</v>
+        <v>7.5000000000000012E-4</v>
       </c>
       <c r="K65" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5000000000000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.6249999999999998E-4</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>10</v>
@@ -3421,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="D66" s="2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="E66" s="2">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>5</v>
@@ -3436,14 +3434,14 @@
         <v>11</v>
       </c>
       <c r="I66" s="3">
-        <v>1.7000000000000001E-3</v>
+        <v>5.8E-4</v>
       </c>
       <c r="J66" s="3">
-        <v>1E-3</v>
+        <v>5.8E-4</v>
       </c>
       <c r="K66" s="3">
-        <f t="shared" si="0"/>
-        <v>4.2500000000000003E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.45E-4</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>10</v>
@@ -3466,10 +3464,10 @@
         <v>9</v>
       </c>
       <c r="D67" s="2">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="E67" s="2">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>5</v>
@@ -3481,14 +3479,14 @@
         <v>11</v>
       </c>
       <c r="I67" s="3">
-        <v>1.0499999999999999E-3</v>
+        <v>5.3000000000000009E-4</v>
       </c>
       <c r="J67" s="3">
-        <v>7.5000000000000012E-4</v>
+        <v>5.3000000000000009E-4</v>
       </c>
       <c r="K67" s="3">
-        <f t="shared" ref="K67:K90" si="1">0.25*I67</f>
-        <v>2.6249999999999998E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.3250000000000002E-4</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>10</v>
@@ -3505,16 +3503,16 @@
         <v>200</v>
       </c>
       <c r="B68" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C68" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D68" s="2">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E68" s="2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>5</v>
@@ -3526,14 +3524,14 @@
         <v>11</v>
       </c>
       <c r="I68" s="3">
-        <v>1.0499999999999999E-3</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="J68" s="3">
-        <v>7.5000000000000012E-4</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="K68" s="3">
         <f t="shared" si="1"/>
-        <v>2.6249999999999998E-4</v>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>10</v>
@@ -3550,16 +3548,16 @@
         <v>200</v>
       </c>
       <c r="B69" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C69" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D69" s="2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="E69" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>5</v>
@@ -3571,14 +3569,14 @@
         <v>11</v>
       </c>
       <c r="I69" s="3">
-        <v>5.8E-4</v>
+        <v>1.8600000000000003E-3</v>
       </c>
       <c r="J69" s="3">
-        <v>5.8E-4</v>
+        <v>1.08E-3</v>
       </c>
       <c r="K69" s="3">
         <f t="shared" si="1"/>
-        <v>1.45E-4</v>
+        <v>4.6500000000000008E-4</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>10</v>
@@ -3595,16 +3593,16 @@
         <v>200</v>
       </c>
       <c r="B70" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C70" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D70" s="2">
-        <v>2.8</v>
+        <v>0.4</v>
       </c>
       <c r="E70" s="2">
-        <v>3</v>
+        <v>0.6</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>5</v>
@@ -3616,14 +3614,14 @@
         <v>11</v>
       </c>
       <c r="I70" s="3">
-        <v>5.3000000000000009E-4</v>
+        <v>4.28E-3</v>
       </c>
       <c r="J70" s="3">
-        <v>5.3000000000000009E-4</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="K70" s="3">
         <f t="shared" si="1"/>
-        <v>1.3250000000000002E-4</v>
+        <v>1.07E-3</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>10</v>
@@ -3646,10 +3644,10 @@
         <v>10</v>
       </c>
       <c r="D71" s="2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E71" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>5</v>
@@ -3661,14 +3659,14 @@
         <v>11</v>
       </c>
       <c r="I71" s="3">
-        <v>1.5800000000000002E-2</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="J71" s="3">
-        <v>6.1000000000000004E-3</v>
+        <v>9.3999999999999997E-4</v>
       </c>
       <c r="K71" s="3">
         <f t="shared" si="1"/>
-        <v>3.9500000000000004E-3</v>
+        <v>5.6749999999999997E-4</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>10</v>
@@ -3691,10 +3689,10 @@
         <v>10</v>
       </c>
       <c r="D72" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E72" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>5</v>
@@ -3706,14 +3704,14 @@
         <v>11</v>
       </c>
       <c r="I72" s="3">
-        <v>1.8600000000000003E-3</v>
+        <v>4.3699999999999998E-3</v>
       </c>
       <c r="J72" s="3">
-        <v>1.08E-3</v>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="K72" s="3">
         <f t="shared" si="1"/>
-        <v>4.6500000000000008E-4</v>
+        <v>1.0924999999999999E-3</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>10</v>
@@ -3736,10 +3734,10 @@
         <v>10</v>
       </c>
       <c r="D73" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E73" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>5</v>
@@ -3751,14 +3749,14 @@
         <v>11</v>
       </c>
       <c r="I73" s="3">
-        <v>4.28E-3</v>
+        <v>1.2200000000000002E-3</v>
       </c>
       <c r="J73" s="3">
-        <v>1.4499999999999999E-3</v>
+        <v>6.2E-4</v>
       </c>
       <c r="K73" s="3">
         <f t="shared" si="1"/>
-        <v>1.07E-3</v>
+        <v>3.0500000000000004E-4</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>10</v>
@@ -3781,10 +3779,10 @@
         <v>10</v>
       </c>
       <c r="D74" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="E74" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>5</v>
@@ -3796,14 +3794,14 @@
         <v>11</v>
       </c>
       <c r="I74" s="3">
-        <v>2.2699999999999999E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="J74" s="3">
-        <v>9.3999999999999997E-4</v>
+        <v>9.2000000000000003E-4</v>
       </c>
       <c r="K74" s="3">
         <f t="shared" si="1"/>
-        <v>5.6749999999999997E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>10</v>
@@ -3826,10 +3824,10 @@
         <v>10</v>
       </c>
       <c r="D75" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="E75" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>5</v>
@@ -3841,14 +3839,14 @@
         <v>11</v>
       </c>
       <c r="I75" s="3">
-        <v>4.3699999999999998E-3</v>
+        <v>3.5000000000000005E-4</v>
       </c>
       <c r="J75" s="3">
-        <v>1.3500000000000001E-3</v>
+        <v>3.5000000000000005E-4</v>
       </c>
       <c r="K75" s="3">
         <f t="shared" si="1"/>
-        <v>1.0924999999999999E-3</v>
+        <v>8.7500000000000013E-5</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>10</v>
@@ -3871,10 +3869,10 @@
         <v>10</v>
       </c>
       <c r="D76" s="2">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="E76" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>5</v>
@@ -3886,14 +3884,14 @@
         <v>11</v>
       </c>
       <c r="I76" s="3">
-        <v>1.2200000000000002E-3</v>
+        <v>3.6999999999999999E-4</v>
       </c>
       <c r="J76" s="3">
-        <v>6.2E-4</v>
+        <v>3.6999999999999999E-4</v>
       </c>
       <c r="K76" s="3">
         <f t="shared" si="1"/>
-        <v>3.0500000000000004E-4</v>
+        <v>9.2499999999999999E-5</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>10</v>
@@ -3916,10 +3914,10 @@
         <v>10</v>
       </c>
       <c r="D77" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="E77" s="2">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>5</v>
@@ -3931,14 +3929,14 @@
         <v>11</v>
       </c>
       <c r="I77" s="3">
-        <v>2.2000000000000001E-3</v>
+        <v>4.2000000000000007E-4</v>
       </c>
       <c r="J77" s="3">
-        <v>9.2000000000000003E-4</v>
+        <v>4.3000000000000004E-4</v>
       </c>
       <c r="K77" s="3">
         <f t="shared" si="1"/>
-        <v>5.5000000000000003E-4</v>
+        <v>1.0500000000000002E-4</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>10</v>
@@ -3961,10 +3959,10 @@
         <v>10</v>
       </c>
       <c r="D78" s="2">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E78" s="2">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>5</v>
@@ -3976,14 +3974,14 @@
         <v>11</v>
       </c>
       <c r="I78" s="3">
-        <v>3.5000000000000005E-4</v>
+        <v>3.8000000000000004E-3</v>
       </c>
       <c r="J78" s="3">
-        <v>3.5000000000000005E-4</v>
+        <v>3.9000000000000003E-3</v>
       </c>
       <c r="K78" s="3">
         <f t="shared" si="1"/>
-        <v>8.7500000000000013E-5</v>
+        <v>9.5000000000000011E-4</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>10</v>
@@ -4000,16 +3998,16 @@
         <v>200</v>
       </c>
       <c r="B79" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C79" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D79" s="2">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E79" s="2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>5</v>
@@ -4021,14 +4019,14 @@
         <v>11</v>
       </c>
       <c r="I79" s="3">
-        <v>3.6999999999999999E-4</v>
+        <v>2.0899999999999998E-3</v>
       </c>
       <c r="J79" s="3">
-        <v>3.6999999999999999E-4</v>
+        <v>2.1200000000000004E-3</v>
       </c>
       <c r="K79" s="3">
         <f t="shared" si="1"/>
-        <v>9.2499999999999999E-5</v>
+        <v>5.2249999999999996E-4</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>10</v>
@@ -4045,16 +4043,16 @@
         <v>200</v>
       </c>
       <c r="B80" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C80" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D80" s="2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="E80" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>5</v>
@@ -4066,14 +4064,14 @@
         <v>11</v>
       </c>
       <c r="I80" s="3">
-        <v>4.2000000000000007E-4</v>
+        <v>1.23E-3</v>
       </c>
       <c r="J80" s="3">
-        <v>4.3000000000000004E-4</v>
+        <v>8.8000000000000003E-4</v>
       </c>
       <c r="K80" s="3">
         <f t="shared" si="1"/>
-        <v>1.0500000000000002E-4</v>
+        <v>3.0749999999999999E-4</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>10</v>
@@ -4090,16 +4088,16 @@
         <v>200</v>
       </c>
       <c r="B81" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C81" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D81" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="E81" s="2">
-        <v>2.4</v>
+        <v>0.6</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>5</v>
@@ -4111,14 +4109,14 @@
         <v>11</v>
       </c>
       <c r="I81" s="3">
-        <v>3.8000000000000004E-3</v>
+        <v>4.2000000000000007E-4</v>
       </c>
       <c r="J81" s="3">
-        <v>3.9000000000000003E-3</v>
+        <v>4.2000000000000007E-4</v>
       </c>
       <c r="K81" s="3">
         <f t="shared" si="1"/>
-        <v>9.5000000000000011E-4</v>
+        <v>1.0500000000000002E-4</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>10</v>
@@ -4141,10 +4139,10 @@
         <v>11</v>
       </c>
       <c r="D82" s="2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E82" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>5</v>
@@ -4156,14 +4154,14 @@
         <v>11</v>
       </c>
       <c r="I82" s="3">
-        <v>2.0899999999999998E-3</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="J82" s="3">
-        <v>2.1200000000000004E-3</v>
+        <v>3.3E-4</v>
       </c>
       <c r="K82" s="3">
         <f t="shared" si="1"/>
-        <v>5.2249999999999996E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>10</v>
@@ -4186,10 +4184,10 @@
         <v>11</v>
       </c>
       <c r="D83" s="2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E83" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>5</v>
@@ -4201,14 +4199,14 @@
         <v>11</v>
       </c>
       <c r="I83" s="3">
-        <v>1.23E-3</v>
+        <v>2.6000000000000003E-4</v>
       </c>
       <c r="J83" s="3">
-        <v>8.8000000000000003E-4</v>
+        <v>2.7E-4</v>
       </c>
       <c r="K83" s="3">
         <f t="shared" si="1"/>
-        <v>3.0749999999999999E-4</v>
+        <v>6.5000000000000008E-5</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>10</v>
@@ -4231,10 +4229,10 @@
         <v>11</v>
       </c>
       <c r="D84" s="2">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E84" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>5</v>
@@ -4246,14 +4244,14 @@
         <v>11</v>
       </c>
       <c r="I84" s="3">
-        <v>4.2000000000000007E-4</v>
+        <v>7.1000000000000002E-4</v>
       </c>
       <c r="J84" s="3">
         <v>4.2000000000000007E-4</v>
       </c>
       <c r="K84" s="3">
         <f t="shared" si="1"/>
-        <v>1.0500000000000002E-4</v>
+        <v>1.775E-4</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>10</v>
@@ -4276,10 +4274,10 @@
         <v>11</v>
       </c>
       <c r="D85" s="2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="E85" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>5</v>
@@ -4291,14 +4289,14 @@
         <v>11</v>
       </c>
       <c r="I85" s="3">
-        <v>3.2000000000000003E-4</v>
+        <v>3.1E-4</v>
       </c>
       <c r="J85" s="3">
-        <v>3.3E-4</v>
+        <v>3.1E-4</v>
       </c>
       <c r="K85" s="3">
         <f t="shared" si="1"/>
-        <v>8.0000000000000007E-5</v>
+        <v>7.75E-5</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>10</v>
@@ -4321,10 +4319,10 @@
         <v>11</v>
       </c>
       <c r="D86" s="2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="E86" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>5</v>
@@ -4336,14 +4334,14 @@
         <v>11</v>
       </c>
       <c r="I86" s="3">
-        <v>2.6000000000000003E-4</v>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="J86" s="3">
-        <v>2.7E-4</v>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="K86" s="3">
         <f t="shared" si="1"/>
-        <v>6.5000000000000008E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>10</v>
@@ -4366,10 +4364,10 @@
         <v>11</v>
       </c>
       <c r="D87" s="2">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="E87" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>5</v>
@@ -4381,14 +4379,14 @@
         <v>11</v>
       </c>
       <c r="I87" s="3">
-        <v>7.1000000000000002E-4</v>
+        <v>6.1000000000000008E-4</v>
       </c>
       <c r="J87" s="3">
-        <v>4.2000000000000007E-4</v>
+        <v>4.6000000000000001E-4</v>
       </c>
       <c r="K87" s="3">
         <f t="shared" si="1"/>
-        <v>1.775E-4</v>
+        <v>1.5250000000000002E-4</v>
       </c>
       <c r="L87" s="1" t="s">
         <v>10</v>
@@ -4397,141 +4395,6 @@
         <v>13</v>
       </c>
       <c r="N87" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="17" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>200</v>
-      </c>
-      <c r="B88" s="2">
-        <v>10</v>
-      </c>
-      <c r="C88" s="2">
-        <v>11</v>
-      </c>
-      <c r="D88" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="E88" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I88" s="3">
-        <v>3.1E-4</v>
-      </c>
-      <c r="J88" s="3">
-        <v>3.1E-4</v>
-      </c>
-      <c r="K88" s="3">
-        <f t="shared" si="1"/>
-        <v>7.75E-5</v>
-      </c>
-      <c r="L88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N88" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" ht="17" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>200</v>
-      </c>
-      <c r="B89" s="2">
-        <v>10</v>
-      </c>
-      <c r="C89" s="2">
-        <v>11</v>
-      </c>
-      <c r="D89" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="E89" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I89" s="3">
-        <v>3.6000000000000002E-4</v>
-      </c>
-      <c r="J89" s="3">
-        <v>3.6000000000000002E-4</v>
-      </c>
-      <c r="K89" s="3">
-        <f t="shared" si="1"/>
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="L89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N89" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" ht="17" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
-        <v>200</v>
-      </c>
-      <c r="B90" s="2">
-        <v>10</v>
-      </c>
-      <c r="C90" s="2">
-        <v>11</v>
-      </c>
-      <c r="D90" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="E90" s="2">
-        <v>2</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I90" s="3">
-        <v>6.1000000000000008E-4</v>
-      </c>
-      <c r="J90" s="3">
-        <v>4.6000000000000001E-4</v>
-      </c>
-      <c r="K90" s="3">
-        <f t="shared" si="1"/>
-        <v>1.5250000000000002E-4</v>
-      </c>
-      <c r="L90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M90" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N90" s="1">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>